<commit_message>
WIP: Redesign of the sensor board.
Major re-design:
- LVDS instead of RS422 driver
- Simplify buck converter design.
- Make the back-plane mostly un-interrupted.
- Smaller cpacitors, eliminate tantal capacitors.
- Make ESD diode smaller.
- Pick different parts.
- Smaller LEDs.
- Eliminate the diodes at the buck converters.
</commit_message>
<xml_diff>
--- a/Doc/Calculation-of-2-section-input-filter.xlsx
+++ b/Doc/Calculation-of-2-section-input-filter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kai_horstmann\Documents\horOpenVario\hovImuBoard\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kai_horstmann\Documents\HorEVario\hovImuBoard\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>fc</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Cin</t>
   </si>
   <si>
-    <t>Input capacitance</t>
-  </si>
-  <si>
     <t>Hz</t>
   </si>
   <si>
@@ -165,6 +162,28 @@
   </si>
   <si>
     <t>Equations below are taken from this document from page 13 onward.</t>
+  </si>
+  <si>
+    <t>Input voltage</t>
+  </si>
+  <si>
+    <t>Input current (est.)</t>
+  </si>
+  <si>
+    <t>Iin</t>
+  </si>
+  <si>
+    <t>Uin</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Input capacitance (
+input capacitors of the step-down converters)</t>
   </si>
 </sst>
 </file>
@@ -208,9 +227,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:H32"/>
+  <dimension ref="C2:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,22 +528,22 @@
   <sheetData>
     <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
@@ -535,12 +557,12 @@
         <v>15000</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
@@ -552,285 +574,313 @@
     </row>
     <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11">
-        <f>12/0.5</f>
-        <v>24</v>
+        <v>48</v>
+      </c>
+      <c r="E11" s="1">
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <f>E11/E12</f>
+        <v>60</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E12">
+      <c r="E14" s="1">
         <f xml:space="preserve"> 44 / 1000 /1000</f>
         <v>4.3999999999999999E-5</v>
       </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14">
-        <f xml:space="preserve"> 100000/(E9 * E9 * E12)</f>
-        <v>0.25586157485438832</v>
-      </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <f xml:space="preserve"> 2.2/1000/1000</f>
-        <v>2.2000000000000001E-6</v>
+        <f xml:space="preserve"> 100000/(E9 * E9 * E14)</f>
+        <v>0.25586157485438832</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17">
-        <f>47/1000/1000</f>
-        <v>4.6999999999999997E-5</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E18">
-        <f>1/(2*PI()*SQRT(E16*E17) )</f>
-        <v>15651.640433668284</v>
+        <f xml:space="preserve"> 4.7/1000/1000</f>
+        <v>4.6999999999999999E-6</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <f>22/1000/1000</f>
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>1/(2*PI()*SQRT(E18*E19) )</f>
+        <v>15651.640433668284</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24">
+        <f xml:space="preserve"> E18/4</f>
+        <v>1.175E-6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24" s="1">
+        <f>E24*1000*1000</f>
+        <v>1.175</v>
+      </c>
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <f xml:space="preserve"> E19/4</f>
+        <v>5.4999999999999999E-6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1">
+        <f>E25*1000*1000</f>
+        <v>5.5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26">
+        <f>1/(2*PI()*SQRT(E24*E25) )</f>
+        <v>62606.561734673138</v>
+      </c>
+      <c r="F26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <f>E26/1000</f>
+        <v>62.606561734673136</v>
+      </c>
+      <c r="H26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22">
-        <f xml:space="preserve"> E16/4</f>
-        <v>5.5000000000000003E-7</v>
-      </c>
-      <c r="F22" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="1">
-        <f>E22*1000*1000</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="H22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23">
-        <f xml:space="preserve"> E17/4</f>
-        <v>1.1749999999999999E-5</v>
-      </c>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1">
-        <f>E23*1000*1000</f>
-        <v>11.75</v>
-      </c>
-      <c r="H23" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28">
+        <f xml:space="preserve"> E24*7</f>
+        <v>8.225E-6</v>
+      </c>
+      <c r="F28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1">
+        <f>E28*1000*1000</f>
+        <v>8.2249999999999996</v>
+      </c>
+      <c r="H28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <f>4*E25</f>
+        <v>2.1999999999999999E-5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1">
+        <f>E29*1000*1000</f>
         <v>22</v>
       </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24">
-        <f>1/(2*PI()*SQRT(E22*E23) )</f>
-        <v>62606.561734673138</v>
-      </c>
-      <c r="F24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24">
-        <f>E24/1000</f>
-        <v>62.606561734673136</v>
-      </c>
-      <c r="H24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26">
-        <f xml:space="preserve"> E22*7</f>
-        <v>3.8500000000000004E-6</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="1">
-        <f>E26*1000*1000</f>
-        <v>3.8500000000000005</v>
-      </c>
-      <c r="H26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27">
-        <f>4*E23</f>
-        <v>4.6999999999999997E-5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="1">
-        <f>E27*1000*1000</f>
-        <v>47</v>
-      </c>
-      <c r="H27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28">
-        <f>1/(2*PI()*SQRT(E26*E27) )</f>
-        <v>11831.52805648269</v>
-      </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28">
-        <f>E28/1000</f>
-        <v>11.831528056482689</v>
-      </c>
-      <c r="H28" t="s">
-        <v>32</v>
+      <c r="H29" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30">
+        <f>1/(2*PI()*SQRT(E28*E29) )</f>
+        <v>11831.52805648269</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30">
+        <f>E30/1000</f>
+        <v>11.831528056482689</v>
+      </c>
+      <c r="H30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="1" t="s">
+      <c r="D33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33">
+        <f>SQRT(E24/E29)</f>
+        <v>0.23110406943429385</v>
+      </c>
+      <c r="F33" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="1">
+        <f>E33*1000</f>
+        <v>231.10406943429385</v>
+      </c>
+      <c r="H33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>39</v>
       </c>
-      <c r="E31">
-        <f>SQRT(E22/E27)</f>
-        <v>0.10817637292669074</v>
-      </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" s="1">
-        <f>E31*1000</f>
-        <v>108.17637292669075</v>
-      </c>
-      <c r="H31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" t="s">
-        <v>40</v>
-      </c>
-      <c r="E32">
-        <f>E22/4</f>
-        <v>1.3750000000000001E-7</v>
-      </c>
-      <c r="G32" s="1">
-        <f>E32*1000*1000</f>
-        <v>0.13750000000000001</v>
-      </c>
-      <c r="H32" t="s">
-        <v>12</v>
+      <c r="E34">
+        <f>E24/4</f>
+        <v>2.9374999999999999E-7</v>
+      </c>
+      <c r="G34" s="1">
+        <f>E34*1000*1000</f>
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>